<commit_message>
Agregegue la nueva automatizacion para las SM
</commit_message>
<xml_diff>
--- a/Automatismo/Automatizaciones/Cancelar task/cancel.xlsx
+++ b/Automatismo/Automatizaciones/Cancelar task/cancel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://falabella-my.sharepoint.com/personal/mbsalasc_tottus_cl/Documents/Escritorio/Developer/Automatismo/Automatizaciones/Cancelar task/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="16" documentId="13_ncr:1_{02E12548-9D77-47F4-9D5F-6AC9C333BD91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A06E1B27-884E-4D20-AB96-64573083274A}"/>
+  <xr:revisionPtr revIDLastSave="37" documentId="13_ncr:1_{02E12548-9D77-47F4-9D5F-6AC9C333BD91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6C6B26C9-26A6-49A8-AED2-02EFCCEC4D22}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{47DFEC38-BB07-4E18-B7E8-A9BF7AF0204D}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4590" uniqueCount="802">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4466" uniqueCount="793">
   <si>
     <t>FECHA_DO</t>
   </si>
@@ -2400,37 +2400,10 @@
     <t>43D4814</t>
   </si>
   <si>
-    <t>RCK12I871</t>
-  </si>
-  <si>
-    <t>12D5212</t>
-  </si>
-  <si>
-    <t>12I2917</t>
-  </si>
-  <si>
-    <t>12I3717</t>
-  </si>
-  <si>
-    <t>12I4715</t>
-  </si>
-  <si>
-    <t>12I4913</t>
-  </si>
-  <si>
-    <t>RCK30D461</t>
-  </si>
-  <si>
-    <t>RCK29I251</t>
-  </si>
-  <si>
-    <t>RCK29I271</t>
-  </si>
-  <si>
-    <t>44D0216</t>
-  </si>
-  <si>
-    <t>44D5017</t>
+    <t>02D3812</t>
+  </si>
+  <si>
+    <t>03I0910</t>
   </si>
 </sst>
 </file>
@@ -3292,10 +3265,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE59C50C-8ED1-4224-B038-760BC62625F3}">
-  <dimension ref="A1:G35"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="A5" sqref="A5:XFD26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3334,42 +3307,42 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
-        <v>46042</v>
+        <v>46044</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>356</v>
+        <v>8</v>
       </c>
       <c r="D2">
-        <v>19099451</v>
+        <v>19192506</v>
       </c>
       <c r="E2" t="s">
-        <v>409</v>
+        <v>791</v>
       </c>
       <c r="F2" t="s">
         <v>10</v>
       </c>
       <c r="G2">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
-        <v>46042</v>
+        <v>46044</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>356</v>
+        <v>8</v>
       </c>
       <c r="D3">
-        <v>19099450</v>
+        <v>19192525</v>
       </c>
       <c r="E3" t="s">
-        <v>373</v>
+        <v>792</v>
       </c>
       <c r="F3" t="s">
         <v>10</v>
@@ -3380,738 +3353,25 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
-        <v>46042</v>
+        <v>46044</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>461</v>
+        <v>8</v>
       </c>
       <c r="D4">
-        <v>19099635</v>
+        <v>19060761</v>
       </c>
       <c r="E4" t="s">
-        <v>792</v>
+        <v>115</v>
       </c>
       <c r="F4" t="s">
         <v>10</v>
       </c>
       <c r="G4">
         <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5" s="1">
-        <v>46042</v>
-      </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" t="s">
-        <v>461</v>
-      </c>
-      <c r="D5">
-        <v>18991988</v>
-      </c>
-      <c r="E5" t="s">
-        <v>509</v>
-      </c>
-      <c r="F5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A6" s="1">
-        <v>46042</v>
-      </c>
-      <c r="B6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" t="s">
-        <v>461</v>
-      </c>
-      <c r="D6">
-        <v>18991982</v>
-      </c>
-      <c r="E6" t="s">
-        <v>517</v>
-      </c>
-      <c r="F6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A7" s="1">
-        <v>46042</v>
-      </c>
-      <c r="B7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" t="s">
-        <v>461</v>
-      </c>
-      <c r="D7">
-        <v>19099643</v>
-      </c>
-      <c r="E7" t="s">
-        <v>793</v>
-      </c>
-      <c r="F7" t="s">
-        <v>10</v>
-      </c>
-      <c r="G7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A8" s="1">
-        <v>46042</v>
-      </c>
-      <c r="B8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" t="s">
-        <v>461</v>
-      </c>
-      <c r="D8">
-        <v>19099859</v>
-      </c>
-      <c r="E8" t="s">
-        <v>791</v>
-      </c>
-      <c r="F8" t="s">
-        <v>10</v>
-      </c>
-      <c r="G8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A9" s="1">
-        <v>46042</v>
-      </c>
-      <c r="B9" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" t="s">
-        <v>461</v>
-      </c>
-      <c r="D9">
-        <v>19099637</v>
-      </c>
-      <c r="E9" t="s">
-        <v>512</v>
-      </c>
-      <c r="F9" t="s">
-        <v>10</v>
-      </c>
-      <c r="G9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A10" s="1">
-        <v>46042</v>
-      </c>
-      <c r="B10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" t="s">
-        <v>461</v>
-      </c>
-      <c r="D10">
-        <v>19099662</v>
-      </c>
-      <c r="E10" t="s">
-        <v>509</v>
-      </c>
-      <c r="F10" t="s">
-        <v>10</v>
-      </c>
-      <c r="G10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A11" s="1">
-        <v>46042</v>
-      </c>
-      <c r="B11" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" t="s">
-        <v>461</v>
-      </c>
-      <c r="D11">
-        <v>19099641</v>
-      </c>
-      <c r="E11" t="s">
-        <v>516</v>
-      </c>
-      <c r="F11" t="s">
-        <v>10</v>
-      </c>
-      <c r="G11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A12" s="1">
-        <v>46042</v>
-      </c>
-      <c r="B12" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12" t="s">
-        <v>461</v>
-      </c>
-      <c r="D12">
-        <v>19099656</v>
-      </c>
-      <c r="E12" t="s">
-        <v>795</v>
-      </c>
-      <c r="F12" t="s">
-        <v>10</v>
-      </c>
-      <c r="G12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A13" s="1">
-        <v>46042</v>
-      </c>
-      <c r="B13" t="s">
-        <v>7</v>
-      </c>
-      <c r="C13" t="s">
-        <v>461</v>
-      </c>
-      <c r="D13">
-        <v>19099631</v>
-      </c>
-      <c r="E13" t="s">
-        <v>523</v>
-      </c>
-      <c r="F13" t="s">
-        <v>10</v>
-      </c>
-      <c r="G13">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A14" s="1">
-        <v>46042</v>
-      </c>
-      <c r="B14" t="s">
-        <v>7</v>
-      </c>
-      <c r="C14" t="s">
-        <v>461</v>
-      </c>
-      <c r="D14">
-        <v>19099858</v>
-      </c>
-      <c r="E14" t="s">
-        <v>475</v>
-      </c>
-      <c r="F14" t="s">
-        <v>10</v>
-      </c>
-      <c r="G14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A15" s="1">
-        <v>46042</v>
-      </c>
-      <c r="B15" t="s">
-        <v>7</v>
-      </c>
-      <c r="C15" t="s">
-        <v>461</v>
-      </c>
-      <c r="D15">
-        <v>19099638</v>
-      </c>
-      <c r="E15" t="s">
-        <v>796</v>
-      </c>
-      <c r="F15" t="s">
-        <v>10</v>
-      </c>
-      <c r="G15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A16" s="1">
-        <v>46042</v>
-      </c>
-      <c r="B16" t="s">
-        <v>7</v>
-      </c>
-      <c r="C16" t="s">
-        <v>461</v>
-      </c>
-      <c r="D16">
-        <v>19099657</v>
-      </c>
-      <c r="E16" t="s">
-        <v>794</v>
-      </c>
-      <c r="F16" t="s">
-        <v>10</v>
-      </c>
-      <c r="G16">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A17" s="1">
-        <v>46042</v>
-      </c>
-      <c r="B17" t="s">
-        <v>7</v>
-      </c>
-      <c r="C17" t="s">
-        <v>461</v>
-      </c>
-      <c r="D17">
-        <v>18991981</v>
-      </c>
-      <c r="E17" t="s">
-        <v>512</v>
-      </c>
-      <c r="F17" t="s">
-        <v>10</v>
-      </c>
-      <c r="G17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A18" s="1">
-        <v>46042</v>
-      </c>
-      <c r="B18" t="s">
-        <v>7</v>
-      </c>
-      <c r="C18" t="s">
-        <v>461</v>
-      </c>
-      <c r="D18">
-        <v>18994036</v>
-      </c>
-      <c r="E18" t="s">
-        <v>554</v>
-      </c>
-      <c r="F18" t="s">
-        <v>10</v>
-      </c>
-      <c r="G18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A19" s="1">
-        <v>46042</v>
-      </c>
-      <c r="B19" t="s">
-        <v>7</v>
-      </c>
-      <c r="C19" t="s">
-        <v>461</v>
-      </c>
-      <c r="D19">
-        <v>18994039</v>
-      </c>
-      <c r="E19" t="s">
-        <v>557</v>
-      </c>
-      <c r="F19" t="s">
-        <v>10</v>
-      </c>
-      <c r="G19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A20" s="1">
-        <v>46042</v>
-      </c>
-      <c r="B20" t="s">
-        <v>7</v>
-      </c>
-      <c r="C20" t="s">
-        <v>461</v>
-      </c>
-      <c r="D20">
-        <v>19099555</v>
-      </c>
-      <c r="E20" t="s">
-        <v>571</v>
-      </c>
-      <c r="F20" t="s">
-        <v>10</v>
-      </c>
-      <c r="G20">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A21" s="1">
-        <v>46042</v>
-      </c>
-      <c r="B21" t="s">
-        <v>7</v>
-      </c>
-      <c r="C21" t="s">
-        <v>461</v>
-      </c>
-      <c r="D21">
-        <v>18991965</v>
-      </c>
-      <c r="E21" t="s">
-        <v>547</v>
-      </c>
-      <c r="F21" t="s">
-        <v>10</v>
-      </c>
-      <c r="G21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A22" s="1">
-        <v>46042</v>
-      </c>
-      <c r="B22" t="s">
-        <v>7</v>
-      </c>
-      <c r="C22" t="s">
-        <v>577</v>
-      </c>
-      <c r="D22">
-        <v>18992023</v>
-      </c>
-      <c r="E22" t="s">
-        <v>623</v>
-      </c>
-      <c r="F22" t="s">
-        <v>10</v>
-      </c>
-      <c r="G22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A23" s="1">
-        <v>46042</v>
-      </c>
-      <c r="B23" t="s">
-        <v>7</v>
-      </c>
-      <c r="C23" t="s">
-        <v>577</v>
-      </c>
-      <c r="D23">
-        <v>19099828</v>
-      </c>
-      <c r="E23" t="s">
-        <v>623</v>
-      </c>
-      <c r="F23" t="s">
-        <v>10</v>
-      </c>
-      <c r="G23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A24" s="1">
-        <v>46042</v>
-      </c>
-      <c r="B24" t="s">
-        <v>7</v>
-      </c>
-      <c r="C24" t="s">
-        <v>577</v>
-      </c>
-      <c r="D24">
-        <v>18992004</v>
-      </c>
-      <c r="E24" t="s">
-        <v>661</v>
-      </c>
-      <c r="F24" t="s">
-        <v>10</v>
-      </c>
-      <c r="G24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A25" s="1">
-        <v>46042</v>
-      </c>
-      <c r="B25" t="s">
-        <v>7</v>
-      </c>
-      <c r="C25" t="s">
-        <v>577</v>
-      </c>
-      <c r="D25">
-        <v>18991998</v>
-      </c>
-      <c r="E25" t="s">
-        <v>676</v>
-      </c>
-      <c r="F25" t="s">
-        <v>10</v>
-      </c>
-      <c r="G25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A26" s="1">
-        <v>46042</v>
-      </c>
-      <c r="B26" t="s">
-        <v>7</v>
-      </c>
-      <c r="C26" t="s">
-        <v>577</v>
-      </c>
-      <c r="D26">
-        <v>19099731</v>
-      </c>
-      <c r="E26" t="s">
-        <v>798</v>
-      </c>
-      <c r="F26" t="s">
-        <v>10</v>
-      </c>
-      <c r="G26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A27" s="1">
-        <v>46042</v>
-      </c>
-      <c r="B27" t="s">
-        <v>7</v>
-      </c>
-      <c r="C27" t="s">
-        <v>577</v>
-      </c>
-      <c r="D27">
-        <v>19099728</v>
-      </c>
-      <c r="E27" t="s">
-        <v>799</v>
-      </c>
-      <c r="F27" t="s">
-        <v>10</v>
-      </c>
-      <c r="G27">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A28" s="1">
-        <v>46042</v>
-      </c>
-      <c r="B28" t="s">
-        <v>7</v>
-      </c>
-      <c r="C28" t="s">
-        <v>577</v>
-      </c>
-      <c r="D28">
-        <v>19099768</v>
-      </c>
-      <c r="E28" t="s">
-        <v>661</v>
-      </c>
-      <c r="F28" t="s">
-        <v>10</v>
-      </c>
-      <c r="G28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A29" s="1">
-        <v>46042</v>
-      </c>
-      <c r="B29" t="s">
-        <v>7</v>
-      </c>
-      <c r="C29" t="s">
-        <v>577</v>
-      </c>
-      <c r="D29">
-        <v>19099804</v>
-      </c>
-      <c r="E29" t="s">
-        <v>627</v>
-      </c>
-      <c r="F29" t="s">
-        <v>10</v>
-      </c>
-      <c r="G29">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A30" s="1">
-        <v>46042</v>
-      </c>
-      <c r="B30" t="s">
-        <v>7</v>
-      </c>
-      <c r="C30" t="s">
-        <v>577</v>
-      </c>
-      <c r="D30">
-        <v>19099817</v>
-      </c>
-      <c r="E30" t="s">
-        <v>633</v>
-      </c>
-      <c r="F30" t="s">
-        <v>10</v>
-      </c>
-      <c r="G30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A31" s="1">
-        <v>46042</v>
-      </c>
-      <c r="B31" t="s">
-        <v>7</v>
-      </c>
-      <c r="C31" t="s">
-        <v>577</v>
-      </c>
-      <c r="D31">
-        <v>19099756</v>
-      </c>
-      <c r="E31" t="s">
-        <v>797</v>
-      </c>
-      <c r="F31" t="s">
-        <v>10</v>
-      </c>
-      <c r="G31">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A32" s="1">
-        <v>46042</v>
-      </c>
-      <c r="B32" t="s">
-        <v>7</v>
-      </c>
-      <c r="C32" t="s">
-        <v>749</v>
-      </c>
-      <c r="D32">
-        <v>19099693</v>
-      </c>
-      <c r="E32" t="s">
-        <v>800</v>
-      </c>
-      <c r="F32" t="s">
-        <v>10</v>
-      </c>
-      <c r="G32">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A33" s="1">
-        <v>46042</v>
-      </c>
-      <c r="B33" t="s">
-        <v>7</v>
-      </c>
-      <c r="C33" t="s">
-        <v>749</v>
-      </c>
-      <c r="D33">
-        <v>19099841</v>
-      </c>
-      <c r="E33" t="s">
-        <v>788</v>
-      </c>
-      <c r="F33" t="s">
-        <v>10</v>
-      </c>
-      <c r="G33">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A34" s="1">
-        <v>46042</v>
-      </c>
-      <c r="B34" t="s">
-        <v>7</v>
-      </c>
-      <c r="C34" t="s">
-        <v>749</v>
-      </c>
-      <c r="D34">
-        <v>19099837</v>
-      </c>
-      <c r="E34" t="s">
-        <v>801</v>
-      </c>
-      <c r="F34" t="s">
-        <v>10</v>
-      </c>
-      <c r="G34">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A35" s="1">
-        <v>46042</v>
-      </c>
-      <c r="B35" t="s">
-        <v>7</v>
-      </c>
-      <c r="C35" t="s">
-        <v>749</v>
-      </c>
-      <c r="D35">
-        <v>18991991</v>
-      </c>
-      <c r="E35" t="s">
-        <v>754</v>
-      </c>
-      <c r="F35" t="s">
-        <v>10</v>
-      </c>
-      <c r="G35">
-        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>